<commit_message>
README in PDF format and touch ups to documentation and folder structure
</commit_message>
<xml_diff>
--- a/notes/miscellaneous/ADC System Overview.xlsx
+++ b/notes/miscellaneous/ADC System Overview.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZM\Desktop\ssmc-infrastructure\ADC drive\ADCS\notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZM\Desktop\ssmc-infrastructure\ADC drive\ADCS\notes\miscellaneous\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B97EA17-75AA-44C6-BB60-CF9F65CBA6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90972B75-95AF-4508-9A34-B35909DF49F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="13176" xr2:uid="{0EF7429A-AB34-4064-9276-5BD80F5A1BAD}"/>
+    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="9463" xr2:uid="{0EF7429A-AB34-4064-9276-5BD80F5A1BAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -49,9 +48,6 @@
     <t>Load Wafers</t>
   </si>
   <si>
-    <t>AXi Machine</t>
-  </si>
-  <si>
     <t>1. Frontside Scan</t>
   </si>
   <si>
@@ -70,9 +66,6 @@
     <t>ADC Server (New Drive)</t>
   </si>
   <si>
-    <t>* AXi Outputs</t>
-  </si>
-  <si>
     <t>1. KLA File</t>
   </si>
   <si>
@@ -103,9 +96,6 @@
     <t>K Drive (Current Drive)</t>
   </si>
   <si>
-    <t>* ADC Outputs</t>
-  </si>
-  <si>
     <t>1. Modified KLA File</t>
   </si>
   <si>
@@ -158,6 +148,15 @@
   </si>
   <si>
     <t>Single-Threaded Edge CLI ADC</t>
+  </si>
+  <si>
+    <t>AVI Machine</t>
+  </si>
+  <si>
+    <t>* AVI Outputs</t>
+  </si>
+  <si>
+    <t>* ADCS Outputs</t>
   </si>
 </sst>
 </file>
@@ -597,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A53D24-771F-464C-A046-FC4E182CEA8E}">
   <dimension ref="B2:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -620,21 +619,21 @@
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="12"/>
       <c r="G2" s="11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="11" t="s">
         <v>18</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>20</v>
       </c>
       <c r="J2" s="9"/>
       <c r="K2" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L2" s="9"/>
     </row>
@@ -646,31 +645,31 @@
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>1</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
@@ -679,19 +678,19 @@
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="1" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="3" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="3"/>
@@ -700,19 +699,19 @@
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
       <c r="D5" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K5" s="4"/>
       <c r="L5" s="3"/>
@@ -721,17 +720,17 @@
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
       <c r="D6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="1"/>
       <c r="I6" s="2"/>
       <c r="J6" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K6" s="4"/>
       <c r="L6" s="3"/>
@@ -740,17 +739,17 @@
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
       <c r="D7" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="1"/>
       <c r="I7" s="2"/>
       <c r="J7" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="3"/>
@@ -761,7 +760,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="2"/>
       <c r="F8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="1"/>
@@ -772,67 +771,67 @@
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F10" s="14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F11" s="14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F12" s="14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F15" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="F16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F19" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F21" s="15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F22" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>